<commit_message>
Last updates and orrder
</commit_message>
<xml_diff>
--- a/Project Outputs for PDN Analyzer/PDN Analyzer.xlsx
+++ b/Project Outputs for PDN Analyzer/PDN Analyzer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Redako-PDNAnalyzer\Project Outputs for PDN Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B36A167-E8E3-48BD-8694-A6B78ADB5E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ECD0A1-8EF4-4407-BB60-7D632E6E6007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10125" yWindow="2760" windowWidth="24780" windowHeight="16005" xr2:uid="{8C8AFBB4-9ADE-4ED2-B7FC-5C2BDE8196F0}"/>
+    <workbookView xWindow="10125" yWindow="2760" windowWidth="24780" windowHeight="16005" xr2:uid="{333E5936-BA8F-4A46-A1BD-2506D2165784}"/>
   </bookViews>
   <sheets>
     <sheet name="PDN Analyzer" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>Designator</t>
   </si>
@@ -51,25 +51,7 @@
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
-    <t>C696814</t>
-  </si>
-  <si>
-    <t>100uF 25V 40mΩ</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4944894</t>
-  </si>
-  <si>
-    <t>470uF 10V 45mΩ</t>
-  </si>
-  <si>
-    <t>C14, C15</t>
+    <t>C16, C17</t>
   </si>
   <si>
     <t>C5246508</t>
@@ -102,7 +84,19 @@
     <t>A2541HWR-2x6P</t>
   </si>
   <si>
-    <t>U1, U4</t>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>C22444686</t>
+  </si>
+  <si>
+    <t>OPA891DR</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>U2, U3</t>
   </si>
   <si>
     <t>C468516</t>
@@ -114,52 +108,70 @@
     <t>Analog Devices</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>C22444686</t>
-  </si>
-  <si>
-    <t>OPA891DR</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C16, C17, C18, C19, C20, C21</t>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>TPS7A3901DSCR</t>
+  </si>
+  <si>
+    <t>C3, C13</t>
   </si>
   <si>
     <t>0402</t>
   </si>
   <si>
+    <t>0.5pF</t>
+  </si>
+  <si>
+    <t>C4, C5, C6, C7, C9, C10, C11, C12, C14, C15, C18, C19, C20, C21, C22, C23</t>
+  </si>
+  <si>
     <t>2.2uF</t>
   </si>
   <si>
-    <t>C22, C23</t>
-  </si>
-  <si>
-    <t>0.5pF</t>
-  </si>
-  <si>
-    <t>R2, R3, R4, R16</t>
+    <t>C24, C25, C28, C30</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>C26, C27, C29</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>R1, R8, R9, R14, R18, R19</t>
+  </si>
+  <si>
+    <t>10kΩ</t>
+  </si>
+  <si>
+    <t>R3, R7, R10, R13</t>
+  </si>
+  <si>
+    <t>1kΩ</t>
+  </si>
+  <si>
+    <t>R4, R6, R11, R12</t>
   </si>
   <si>
     <t>100Ω</t>
   </si>
   <si>
-    <t>R7, R8, R12, R13</t>
-  </si>
-  <si>
-    <t>1kΩ</t>
-  </si>
-  <si>
-    <t>R9, R10, R11, R14</t>
-  </si>
-  <si>
-    <t>10kΩ</t>
-  </si>
-  <si>
-    <t>R1</t>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>11kΩ</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>21kΩ</t>
+  </si>
+  <si>
+    <t>R2</t>
   </si>
   <si>
     <t>0603</t>
@@ -168,10 +180,16 @@
     <t>0.5Ω</t>
   </si>
   <si>
-    <t>R5, R6, R15</t>
-  </si>
-  <si>
     <t>0Ω</t>
+  </si>
+  <si>
+    <t>C2685819</t>
+  </si>
+  <si>
+    <t>R15, R16</t>
+  </si>
+  <si>
+    <t>R5</t>
   </si>
 </sst>
 </file>
@@ -547,10 +565,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CD954B-8E61-4541-BCBE-21BC815F534C}">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE712ACA-5342-48F7-9D09-26D2ADB0FB96}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -599,237 +619,329 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>16</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1">
         <v>4</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>